<commit_message>
add socket and update simulation method
</commit_message>
<xml_diff>
--- a/media/1/PMP-Données.xlsx
+++ b/media/1/PMP-Données.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEA3394-9DF5-4071-B088-88558C200D39}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" tabRatio="565"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" tabRatio="565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -128,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
@@ -658,55 +659,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E81EA45-5640-4586-BB63-8E98B1379CD2}">
   <dimension ref="A1:AA42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="42.28515625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" style="15" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
-    <col min="6" max="10" width="27.140625" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" customWidth="1"/>
-    <col min="13" max="13" width="24.42578125" customWidth="1"/>
-    <col min="14" max="17" width="27.140625" customWidth="1"/>
-    <col min="18" max="18" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.5703125" customWidth="1"/>
-    <col min="20" max="20" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.42578125" customWidth="1"/>
-    <col min="22" max="22" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="6" max="10" width="27.109375" customWidth="1"/>
+    <col min="11" max="11" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.109375" customWidth="1"/>
+    <col min="13" max="13" width="24.44140625" customWidth="1"/>
+    <col min="14" max="17" width="27.109375" customWidth="1"/>
+    <col min="18" max="18" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.5546875" customWidth="1"/>
+    <col min="20" max="20" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.44140625" customWidth="1"/>
+    <col min="22" max="22" width="22.44140625" customWidth="1"/>
     <col min="23" max="23" width="22" customWidth="1"/>
-    <col min="24" max="24" width="18.140625" customWidth="1"/>
-    <col min="25" max="26" width="17.85546875" customWidth="1"/>
-    <col min="27" max="27" width="14.42578125" customWidth="1"/>
-    <col min="28" max="28" width="14.85546875" customWidth="1"/>
-    <col min="29" max="29" width="16.5703125" customWidth="1"/>
-    <col min="30" max="30" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.109375" customWidth="1"/>
+    <col min="25" max="26" width="17.88671875" customWidth="1"/>
+    <col min="27" max="27" width="14.44140625" customWidth="1"/>
+    <col min="28" max="28" width="14.88671875" customWidth="1"/>
+    <col min="29" max="29" width="16.5546875" customWidth="1"/>
+    <col min="30" max="30" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="33" max="35" width="13" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="22"/>
     </row>
-    <row r="2" spans="1:27" s="7" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:27" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D3" s="26" t="s">
         <v>2</v>
       </c>
@@ -739,7 +740,7 @@
       <c r="Z3" s="20"/>
       <c r="AA3" s="20"/>
     </row>
-    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>1</v>
       </c>
@@ -797,7 +798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:27" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="23"/>
       <c r="C5" s="7"/>
       <c r="D5" s="25"/>
@@ -840,7 +841,7 @@
       </c>
       <c r="AA5" s="29"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>1</v>
       </c>
@@ -913,7 +914,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -986,7 +987,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="9">
         <v>3</v>
       </c>
@@ -1060,7 +1061,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -1133,7 +1134,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>5</v>
       </c>
@@ -1206,7 +1207,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -1280,7 +1281,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>7</v>
       </c>
@@ -1353,7 +1354,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>8</v>
       </c>
@@ -1426,7 +1427,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="9">
         <v>9</v>
       </c>
@@ -1500,7 +1501,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>10</v>
       </c>
@@ -1573,7 +1574,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>11</v>
       </c>
@@ -1646,7 +1647,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="9">
         <v>12</v>
       </c>
@@ -1720,7 +1721,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>13</v>
       </c>
@@ -1793,7 +1794,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>14</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="9">
         <v>15</v>
       </c>
@@ -1940,7 +1941,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>16</v>
       </c>
@@ -2013,7 +2014,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>17</v>
       </c>
@@ -2086,7 +2087,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="9">
         <v>18</v>
       </c>
@@ -2160,7 +2161,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>19</v>
       </c>
@@ -2233,7 +2234,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <v>20</v>
       </c>
@@ -2306,7 +2307,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="9">
         <v>21</v>
       </c>
@@ -2380,7 +2381,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>22</v>
       </c>
@@ -2453,7 +2454,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <v>23</v>
       </c>
@@ -2526,7 +2527,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="9">
         <v>24</v>
       </c>
@@ -2600,7 +2601,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>25</v>
       </c>
@@ -2673,7 +2674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <v>26</v>
       </c>
@@ -2746,7 +2747,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <v>27</v>
       </c>
@@ -2819,7 +2820,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <v>28</v>
       </c>
@@ -2892,7 +2893,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <v>29</v>
       </c>
@@ -2965,7 +2966,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" s="9">
         <v>30</v>
       </c>
@@ -3038,7 +3039,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" s="9">
         <v>31</v>
       </c>
@@ -3111,7 +3112,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D39" s="20" t="s">
         <v>0</v>
       </c>
@@ -3122,7 +3123,7 @@
       <c r="I39" s="20"/>
       <c r="J39" s="20"/>
     </row>
-    <row r="40" spans="1:27" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="17" t="s">
         <v>9</v>
       </c>
@@ -3148,7 +3149,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B41" s="18" t="s">
         <v>32</v>
       </c>
@@ -3174,7 +3175,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B42" s="19"/>
       <c r="C42" s="3"/>
       <c r="D42" s="4"/>

</xml_diff>